<commit_message>
Added param values for sl_bt_scanner_set_mode() and sl_bt_scanner_set_timing().
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -94,10 +94,19 @@
     <t>sl_bt_scanner_set_mode()</t>
   </si>
   <si>
+    <t>Set phy to 1M and mode to passive scanning</t>
+  </si>
+  <si>
     <t>sl_bt_scanner_set_timing()</t>
   </si>
   <si>
+    <t>Set phy to 1M, scan interval to 50ms and scan window to 25ms</t>
+  </si>
+  <si>
     <t>sl_bt_connection_set_default_parameters()</t>
+  </si>
+  <si>
+    <t>See the assignment document for these values</t>
   </si>
   <si>
     <t>sl_bt_scanner_start()</t>
@@ -136,30 +145,7 @@
     <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Do not build your state machine into your  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>handle_ble_event()</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> function! Instead build a new state machine for A7. </t>
-    </r>
+    <t xml:space="preserve">Do not build your state machine into your  handle_ble_event() function! Instead build a new state machine for A7. </t>
   </si>
   <si>
     <t>sl_bt_evt_gatt_service_id</t>
@@ -189,7 +175,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -234,11 +220,6 @@
     <font>
       <sz val="12"/>
       <color indexed="14"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="15"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -352,7 +333,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -398,7 +379,7 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -407,7 +388,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -421,9 +402,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,7 +426,6 @@
       <rgbColor rgb="ff2236ff"/>
       <rgbColor rgb="ff4d8f72"/>
       <rgbColor rgb="ff4d8f72"/>
-      <rgbColor rgb="ff2e74b5"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1612,7 +1589,9 @@
       <c r="E7" t="s" s="17">
         <v>14</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" t="s" s="15">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" ht="13.75" customHeight="1">
       <c r="A8" s="7"/>
@@ -1620,9 +1599,11 @@
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="F8" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="F8" t="s" s="18">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="7"/>
@@ -1630,9 +1611,11 @@
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" t="s" s="17">
-        <v>16</v>
-      </c>
-      <c r="F9" s="19"/>
+        <v>18</v>
+      </c>
+      <c r="F9" t="s" s="15">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" ht="26.75" customHeight="1">
       <c r="A10" s="7"/>
@@ -1640,10 +1623,10 @@
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" t="s" s="17">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s" s="15">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" ht="13.55" customHeight="1">
@@ -1657,7 +1640,7 @@
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" t="s" s="20">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -1675,7 +1658,7 @@
     <row r="14" ht="13.55" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" t="s" s="20">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1693,12 +1676,12 @@
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" t="s" s="20">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" t="s" s="21">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F16" s="19"/>
     </row>
@@ -1712,7 +1695,7 @@
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" t="s" s="10">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="19"/>
@@ -1723,12 +1706,12 @@
     <row r="19" ht="78.75" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" t="s" s="20">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" t="s" s="21">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F19" s="19"/>
     </row>
@@ -1743,15 +1726,15 @@
     <row r="21" ht="39.75" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" t="s" s="20">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" t="s" s="21">
-        <v>27</v>
-      </c>
-      <c r="F21" t="s" s="23">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="F21" t="s" s="15">
+        <v>31</v>
       </c>
     </row>
     <row r="22" ht="13.55" customHeight="1">
@@ -1765,12 +1748,12 @@
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" t="s" s="20">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" t="s" s="21">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F23" s="19"/>
     </row>
@@ -1785,12 +1768,12 @@
     <row r="25" ht="13.55" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" t="s" s="20">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
       <c r="E25" t="s" s="21">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F25" s="19"/>
     </row>
@@ -1805,12 +1788,12 @@
     <row r="27" ht="65.75" customHeight="1">
       <c r="A27" s="7"/>
       <c r="B27" t="s" s="20">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" t="s" s="21">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F27" s="19"/>
     </row>

</xml_diff>

<commit_message>
Assignment6 by tharuni gelli
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharu\SimplicityStudio\v5_workspace\ecen5823-assignment6-tharuni-gelli\questions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4C5BC0-A6CD-4C6F-9F32-6EBE45963CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -27,7 +36,7 @@
   <si>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -54,7 +63,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -88,33 +97,18 @@
     <t>This event is generated on stack boot up</t>
   </si>
   <si>
-    <t xml:space="preserve">You can also document in column D values that need to be saved in response to receiving BT stack events. </t>
-  </si>
-  <si>
     <t>sl_bt_scanner_set_mode()</t>
   </si>
   <si>
-    <t>Set phy to 1M and mode to passive scanning</t>
-  </si>
-  <si>
     <t>sl_bt_scanner_set_timing()</t>
   </si>
   <si>
-    <t>Set phy to 1M, scan interval to 50ms and scan window to 25ms</t>
-  </si>
-  <si>
     <t>sl_bt_connection_set_default_parameters()</t>
   </si>
   <si>
-    <t>See the assignment document for these values</t>
-  </si>
-  <si>
     <t>sl_bt_scanner_start()</t>
   </si>
   <si>
-    <t>You should start and stop scanning just like you did with advertising for a Server.</t>
-  </si>
-  <si>
     <t>sl_bt_evt_connection_opened_id</t>
   </si>
   <si>
@@ -124,67 +118,118 @@
     <t>sl_bt_evt_system_soft_timer_id</t>
   </si>
   <si>
-    <t>This event indicates that a soft timer has expired.</t>
-  </si>
-  <si>
     <t>Events only for Masters/Clients</t>
   </si>
   <si>
     <t>sl_bt_evt_scanner_scan_report_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_procedure_completed_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_service_id</t>
+  </si>
+  <si>
+    <t>A GATT service in the remote GATT database was discovered</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_characteristic_id</t>
+  </si>
+  <si>
+    <t>sl_bt_advertiser_create_set()</t>
+  </si>
+  <si>
+    <t>sl_bt_advertiser_set_timing()</t>
+  </si>
+  <si>
+    <t>sl_bt_advertiser_start()</t>
+  </si>
+  <si>
+    <t>sl_bt_system_get_identity_address()</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>sl_bt_advertiser_stop()</t>
+  </si>
+  <si>
+    <t>Connection is opened</t>
+  </si>
+  <si>
+    <t>Save connection handle</t>
+  </si>
+  <si>
+    <t>sl_bt_connection_set_parameters()</t>
+  </si>
+  <si>
+    <t>Connetion is closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sl_bt_scanner_stop()</t>
   </si>
   <si>
     <t>Received for advertising or scan response packets generated by: sl_bt_scanner_start().
 Is the bd_addr, packet_type and address_type what we expect for our Server? If yes:
    sl_bt_scanner_stop()
-   sl_bt_connection_open()</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_procedure_completed_id</t>
-  </si>
-  <si>
-    <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do not build your state machine into your  handle_ble_event() function! Instead build a new state machine for A7. </t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_service_id</t>
-  </si>
-  <si>
-    <t>A GATT service in the remote GATT database was discovered</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_characteristic_id</t>
-  </si>
-  <si>
-    <t>A GATT characteristic in the remote GATT database was discovered</t>
+   sl_bt_connection_open(). We connect server and client after getting this event.</t>
+  </si>
+  <si>
+    <t>sl_bt_connection_open()</t>
+  </si>
+  <si>
+    <t>Save service Handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save characteristic handle and properties. </t>
+  </si>
+  <si>
+    <t>This event is generated after issuing either the   sl_bt_gatt_discover_characteristics or  sl_bt_gatt_discover_characteristics_by_uuid command.</t>
+  </si>
+  <si>
+    <t>We discovered GATT characteristics.</t>
+  </si>
+  <si>
+    <t>All these functions are same as we did in the previous assignment</t>
+  </si>
+  <si>
+    <t>Soft timer expiration is indicated by this evevnt</t>
+  </si>
+  <si>
+    <t>Upon receiving this event signaling the readiness to execute the next GATT command, it is advisable to diligently inspect any returned error codes. Integrating this event into the sequence of your new state machine can enhance its efficiency and reliability. It is recommended to preserve the GATT command status by storing it in a boolean variable at this juncture, facilitating subsequent GATT command calls with confidence.</t>
   </si>
   <si>
     <t>sl_bt_evt_gatt_characteristic_value_id</t>
   </si>
   <si>
-    <t>If an indication or notification has been enabled for a characteristic, this event is triggered whenever an indication or notification is received from the remote GATT server.
-Is the characteristic handle and att_opcode we expect? If yes: 
-   sl_bt_gatt_send_characteristic_confirmation()</t>
+    <t xml:space="preserve">Save opcode and characteristic values. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sl_bt_gatt_send_characteristic_confirmation(). </t>
+  </si>
+  <si>
+    <t>Bubble diagram for A7</t>
+  </si>
+  <si>
+    <t>When an indication or notification is enabled for a characteristic, the corresponding event is triggered each time a similar indication or notification is received from the remote GATT server.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="13"/>
@@ -197,7 +242,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -213,17 +258,32 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="14"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="14"/>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +296,25 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -312,127 +389,242 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff2236ff"/>
-      <rgbColor rgb="ff4d8f72"/>
-      <rgbColor rgb="ff4d8f72"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF2236FF"/>
+      <rgbColor rgb="FF4D8F72"/>
+      <rgbColor rgb="FF4D8F72"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2270376</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>75114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D973049-EE90-6085-6291-A95FB41B1391}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="20161250"/>
+          <a:ext cx="7429751" cy="5440864"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -634,7 +826,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -653,7 +845,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -683,7 +875,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -709,7 +901,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -735,7 +927,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -761,7 +953,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -787,7 +979,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -813,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -839,7 +1031,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -865,7 +1057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -891,7 +1083,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,9 +1096,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -923,7 +1121,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -942,7 +1140,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -968,7 +1166,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -994,7 +1192,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1020,7 +1218,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1046,7 +1244,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1072,7 +1270,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1098,7 +1296,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1124,7 +1322,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1150,7 +1348,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1176,7 +1374,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,9 +1387,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1205,7 +1409,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1224,7 +1428,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1254,7 +1458,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1280,7 +1484,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1306,7 +1510,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1332,7 +1536,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1358,7 +1562,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1384,7 +1588,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1410,7 +1614,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1436,7 +1640,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1462,7 +1666,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1475,352 +1679,493 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="48" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.8516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.55" customHeight="1">
+    <row r="1" spans="1:7" ht="14.55" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" ht="12.05" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" ht="119.55" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" t="s" s="9">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" ht="12" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="119.55" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s" s="9">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" ht="12.05" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s" s="6">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="12" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="9">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="9">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s" s="9">
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" ht="13.75" customHeight="1">
-      <c r="A5" t="s" s="10">
+    <row r="5" spans="1:7" ht="13.8" customHeight="1">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="26.7" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" ht="26.75" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" t="s" s="11">
+      <c r="B6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" t="s" s="14">
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s" s="15">
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A7" s="4"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" t="s" s="17">
+      <c r="F7" s="23"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="13.8" customHeight="1">
+      <c r="A8" s="4"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s" s="15">
+      <c r="F8" s="23"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" ht="38.4" customHeight="1">
+      <c r="A9" s="4"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" ht="13.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" t="s" s="17">
+      <c r="F9" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="26.7" customHeight="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F8" t="s" s="18">
+      <c r="F10" s="23"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" ht="13.2" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="13.2" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="13.2" customHeight="1">
+      <c r="A13" s="4"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" ht="13.2" customHeight="1">
+      <c r="A14" s="4"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A15" s="4"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A16" s="4"/>
+      <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" t="s" s="17">
+      <c r="C16" s="17"/>
+      <c r="D16" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A17" s="4"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="19"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" ht="13.5" customHeight="1">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" ht="78.75" customHeight="1">
+      <c r="A19" s="4"/>
+      <c r="B19" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s" s="15">
+      <c r="C19" s="24"/>
+      <c r="D19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:7" ht="39.75" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" ht="26.75" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" t="s" s="17">
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A22" s="4"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:7" ht="13.5" customHeight="1">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" ht="196.8" customHeight="1">
+      <c r="A24" s="7"/>
+      <c r="B24" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:7" ht="22.8" customHeight="1">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s" s="15">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" t="s" s="20">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="1:7" ht="179.4" customHeight="1">
+      <c r="A27" s="4"/>
+      <c r="B27" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" t="s" s="20">
+      <c r="C27" s="17"/>
+      <c r="D27" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A28" s="4"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A29" s="4"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A30" s="4"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="16"/>
+    </row>
+    <row r="31" spans="1:7" ht="76.8" customHeight="1">
+      <c r="A31" s="4"/>
+      <c r="B31" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" t="s" s="20">
+      <c r="C31" s="24"/>
+      <c r="D31" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" t="s" s="21">
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A32" s="4"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="1:7" ht="127.2" customHeight="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="19"/>
-    </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-    </row>
-    <row r="19" ht="78.75" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" t="s" s="20">
-        <v>27</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" t="s" s="21">
-        <v>28</v>
-      </c>
-      <c r="F19" s="19"/>
-    </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="19"/>
-    </row>
-    <row r="21" ht="39.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" t="s" s="20">
-        <v>29</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" t="s" s="21">
-        <v>30</v>
-      </c>
-      <c r="F21" t="s" s="15">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" t="s" s="20">
-        <v>32</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" t="s" s="21">
-        <v>33</v>
-      </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" t="s" s="20">
-        <v>34</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" t="s" s="21">
-        <v>35</v>
-      </c>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-    </row>
-    <row r="27" ht="65.75" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" t="s" s="20">
-        <v>36</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" t="s" s="21">
-        <v>37</v>
-      </c>
-      <c r="F27" s="19"/>
-    </row>
-    <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" ht="40.200000000000003" customHeight="1">
+      <c r="A34" s="4"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="16"/>
+    </row>
+    <row r="35" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A35" s="4"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="1:7" ht="228" customHeight="1">
+      <c r="A36" s="4"/>
+      <c r="B36" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="16"/>
+    </row>
+    <row r="37" spans="1:7" ht="13.5" customHeight="1">
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
+      <c r="E37"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="39" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final A7 submission by tharuni gelli
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharu\SimplicityStudio\v5_workspace\ecen5823-assignment6-tharuni-gelli\questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharu\SimplicityStudio\v5_workspace\ecen5823-assignment7-tharuni-gelli\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4C5BC0-A6CD-4C6F-9F32-6EBE45963CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2609A733-AEFA-4643-A54A-74193DBD95F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -136,100 +136,116 @@
     <t>sl_bt_evt_gatt_characteristic_id</t>
   </si>
   <si>
-    <t>sl_bt_advertiser_create_set()</t>
-  </si>
-  <si>
-    <t>sl_bt_advertiser_set_timing()</t>
-  </si>
-  <si>
-    <t>sl_bt_advertiser_start()</t>
-  </si>
-  <si>
-    <t>sl_bt_system_get_identity_address()</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>sl_bt_advertiser_stop()</t>
-  </si>
-  <si>
-    <t>Connection is opened</t>
-  </si>
-  <si>
-    <t>Save connection handle</t>
-  </si>
-  <si>
-    <t>sl_bt_connection_set_parameters()</t>
-  </si>
-  <si>
-    <t>Connetion is closed</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sl_bt_scanner_stop()</t>
+    <t>sl_bt_connection_open()</t>
+  </si>
+  <si>
+    <t>Save service Handle</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_gatt_characteristic_value_id</t>
+  </si>
+  <si>
+    <t>Bubble diagram for A7</t>
+  </si>
+  <si>
+    <t>Set phy to 1M and mode to passive scanning</t>
+  </si>
+  <si>
+    <t>Set phy to 1M, scan interval to 50ms and scan window to 25ms</t>
+  </si>
+  <si>
+    <t>See the assignment document for these values</t>
+  </si>
+  <si>
+    <t>You should start and stop scanning just like you did with advertising for a Server.</t>
+  </si>
+  <si>
+    <t>displayInit()</t>
+  </si>
+  <si>
+    <t>Initializes the LCD screen</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_discover_primary_services_by_uuid()</t>
+  </si>
+  <si>
+    <t>Initiates search for primary services in GATT database with specific UUID(save connection handle)</t>
+  </si>
+  <si>
+    <t>Initiates scanning for advertising devices with chosen discovery mode</t>
+  </si>
+  <si>
+    <t>This event indicates that a soft timer has expired.</t>
+  </si>
+  <si>
+    <t>displayUpdate()</t>
   </si>
   <si>
     <t>Received for advertising or scan response packets generated by: sl_bt_scanner_start().
 Is the bd_addr, packet_type and address_type what we expect for our Server? If yes:
    sl_bt_scanner_stop()
-   sl_bt_connection_open(). We connect server and client after getting this event.</t>
-  </si>
-  <si>
-    <t>sl_bt_connection_open()</t>
-  </si>
-  <si>
-    <t>Save service Handle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save characteristic handle and properties. </t>
-  </si>
-  <si>
-    <t>This event is generated after issuing either the   sl_bt_gatt_discover_characteristics or  sl_bt_gatt_discover_characteristics_by_uuid command.</t>
-  </si>
-  <si>
-    <t>We discovered GATT characteristics.</t>
-  </si>
-  <si>
-    <t>All these functions are same as we did in the previous assignment</t>
-  </si>
-  <si>
-    <t>Soft timer expiration is indicated by this evevnt</t>
-  </si>
-  <si>
-    <t>Upon receiving this event signaling the readiness to execute the next GATT command, it is advisable to diligently inspect any returned error codes. Integrating this event into the sequence of your new state machine can enhance its efficiency and reliability. It is recommended to preserve the GATT command status by storing it in a boolean variable at this juncture, facilitating subsequent GATT command calls with confidence.</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_gatt_characteristic_value_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save opcode and characteristic values. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sl_bt_gatt_send_characteristic_confirmation(). </t>
-  </si>
-  <si>
-    <t>Bubble diagram for A7</t>
-  </si>
-  <si>
-    <t>When an indication or notification is enabled for a characteristic, the corresponding event is triggered each time a similar indication or notification is received from the remote GATT server.</t>
+   sl_bt_connection_open()</t>
+  </si>
+  <si>
+    <t>sl_bt_scanner_stop()</t>
+  </si>
+  <si>
+    <t>Stops the scanning process</t>
+  </si>
+  <si>
+    <t>Initiates connection to a BLE device establishing a BLE link for communication</t>
+  </si>
+  <si>
+    <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not build your state machine into your  handle_ble_event() function! Instead build a new state machine for A7. </t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_discover_characteristics_by_uuid()</t>
+  </si>
+  <si>
+    <t>Initiates a search for GATT characteristics with the specific UUID within the GATT database</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_set_characteristics_notfication()</t>
+  </si>
+  <si>
+    <t>Enables/disables notifications for a apecific GATT characteristic</t>
+  </si>
+  <si>
+    <t>Save characteristic Handle and properties</t>
+  </si>
+  <si>
+    <t>A GATT characteristic in the remote GATT database was discovered</t>
+  </si>
+  <si>
+    <t>Save opcode and characteristic values</t>
+  </si>
+  <si>
+    <t>If an indication or notification has been enabled for a characteristic, this event is triggered whenever an indication or notification is received from the remote GATT server.
+Is the characteristic handle and att_opcode we expect? If yes: 
+   sl_bt_gatt_send_characteristic_confirmation()</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_send_characteristic_confirmation()</t>
+  </si>
+  <si>
+    <t>Send confirmation in response to an indication from a characteristic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="13"/>
@@ -258,32 +274,28 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="10"/>
+      <color indexed="14"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color indexed="14"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,25 +308,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -389,102 +384,137 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,22 +603,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>1254125</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2270376</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>75114</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2901950</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>49334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D973049-EE90-6085-6291-A95FB41B1391}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC8DF319-808C-7981-28B7-CBABFB5E3BB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -610,8 +640,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="666750" y="20161250"/>
-          <a:ext cx="7429751" cy="5440864"/>
+          <a:off x="1254125" y="20637499"/>
+          <a:ext cx="8651875" cy="6335835"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1701,460 +1731,441 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="48" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="52.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="85.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="89.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.55" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:7" ht="12" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" ht="119.55" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="119.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="12" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.8" customHeight="1">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:7" ht="26.7" customHeight="1">
-      <c r="A6" s="7" t="s">
+    <row r="5" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" ht="26.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="23" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21" t="s">
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" ht="13.8" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="21" t="s">
+      <c r="F7" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" ht="38.4" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="21" t="s">
+      <c r="F8" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="20"/>
+      <c r="F23" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="315" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" ht="26.7" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" ht="13.2" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="21" t="s">
+      <c r="F24" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="198.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" ht="314.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="269.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" ht="13.2" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" ht="13.2" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="21" t="s">
+      <c r="E28" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="248.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" ht="13.2" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21" t="s">
+      <c r="E31" s="21"/>
+      <c r="F31" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="1:6" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="12"/>
+    </row>
+    <row r="35" spans="1:6" ht="206.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
+      <c r="B35" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18" t="s">
+      <c r="C35" s="12"/>
+      <c r="D35" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="396" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="32"/>
+    </row>
+    <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" ht="78.75" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" ht="39.75" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" ht="196.8" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:7" ht="22.8" customHeight="1">
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:7" ht="179.4" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:7" ht="76.8" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="24"/>
-      <c r="F31" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="1:7" ht="127.2" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="1:7" ht="40.200000000000003" customHeight="1">
-      <c r="A34" s="4"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G34" s="16"/>
-    </row>
-    <row r="35" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A35" s="4"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="1:7" ht="228" customHeight="1">
-      <c r="A36" s="4"/>
-      <c r="B36" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="16"/>
-    </row>
-    <row r="37" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="14"/>
-      <c r="E37"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="39" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>